<commit_message>
okay it works, might change the layout later
</commit_message>
<xml_diff>
--- a/output/release_CEREZA_V1.4.2.xlsx
+++ b/output/release_CEREZA_V1.4.2.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,10 +470,15 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Merge Requests</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Created At</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Updated At</t>
         </is>
@@ -508,10 +513,15 @@
           <t>Hook up the logfile to textstream and socket at the same time ?</t>
         </is>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Resolve "Can we post the log on a port through a socket ?"</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>45986.59277880787</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="I2" s="2" t="n">
         <v>46014.48094136574</v>
       </c>
     </row>
@@ -689,10 +699,15 @@
 Remove extensive logging and cleanup before merging on main</t>
         </is>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Draft: Resolve "Problem after 24H"; Resolve "Problem after 24H"</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
         <v>45978.50888179398</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="2" t="n">
         <v>46014.48102471065</v>
       </c>
     </row>

</xml_diff>